<commit_message>
Added some DNA sequences
</commit_message>
<xml_diff>
--- a/data/Primers template.xlsx
+++ b/data/Primers template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loa012\Python\PYEAST\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7304768-ABA2-4AE5-A10C-BDD0A5F191D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222E8D0B-6E19-451B-B4BC-FB822C26237C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{3674F192-AC5C-47E2-8A02-E860BFF3F7B0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
     <t>Plate or Box ID</t>
   </si>
@@ -48,6 +48,294 @@
   </si>
   <si>
     <t>Sequence</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>A7</t>
+  </si>
+  <si>
+    <t>A8</t>
+  </si>
+  <si>
+    <t>A9</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>A11</t>
+  </si>
+  <si>
+    <t>A12</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>B6</t>
+  </si>
+  <si>
+    <t>B7</t>
+  </si>
+  <si>
+    <t>B8</t>
+  </si>
+  <si>
+    <t>B9</t>
+  </si>
+  <si>
+    <t>B10</t>
+  </si>
+  <si>
+    <t>B11</t>
+  </si>
+  <si>
+    <t>B12</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>D9</t>
+  </si>
+  <si>
+    <t>D10</t>
+  </si>
+  <si>
+    <t>D11</t>
+  </si>
+  <si>
+    <t>D12</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>E6</t>
+  </si>
+  <si>
+    <t>E7</t>
+  </si>
+  <si>
+    <t>E8</t>
+  </si>
+  <si>
+    <t>E9</t>
+  </si>
+  <si>
+    <t>E10</t>
+  </si>
+  <si>
+    <t>E11</t>
+  </si>
+  <si>
+    <t>E12</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>F5</t>
+  </si>
+  <si>
+    <t>F6</t>
+  </si>
+  <si>
+    <t>F7</t>
+  </si>
+  <si>
+    <t>F8</t>
+  </si>
+  <si>
+    <t>F9</t>
+  </si>
+  <si>
+    <t>F10</t>
+  </si>
+  <si>
+    <t>F11</t>
+  </si>
+  <si>
+    <t>F12</t>
+  </si>
+  <si>
+    <t>G1</t>
+  </si>
+  <si>
+    <t>G2</t>
+  </si>
+  <si>
+    <t>G3</t>
+  </si>
+  <si>
+    <t>G4</t>
+  </si>
+  <si>
+    <t>G5</t>
+  </si>
+  <si>
+    <t>G6</t>
+  </si>
+  <si>
+    <t>G7</t>
+  </si>
+  <si>
+    <t>G8</t>
+  </si>
+  <si>
+    <t>G9</t>
+  </si>
+  <si>
+    <t>G10</t>
+  </si>
+  <si>
+    <t>G11</t>
+  </si>
+  <si>
+    <t>G12</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>H3</t>
+  </si>
+  <si>
+    <t>H4</t>
+  </si>
+  <si>
+    <t>H5</t>
+  </si>
+  <si>
+    <t>H6</t>
+  </si>
+  <si>
+    <t>H7</t>
+  </si>
+  <si>
+    <t>H8</t>
+  </si>
+  <si>
+    <t>H9</t>
+  </si>
+  <si>
+    <t>H10</t>
+  </si>
+  <si>
+    <t>H11</t>
+  </si>
+  <si>
+    <t>H12</t>
   </si>
 </sst>
 </file>
@@ -451,10 +739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02F98113-4DF1-41D8-8ACA-74C6010B1D34}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B2" sqref="B2:B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -479,6 +767,486 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B38" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B39" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B41" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B42" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B44" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B45" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B46" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B47" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B48" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B49" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B50" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B51" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B52" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B53" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B54" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B55" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B56" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B57" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B58" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B59" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B60" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B61" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B62" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B63" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B64" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B65" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B66" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B67" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B68" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B69" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B70" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B71" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B72" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B73" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B74" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B75" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B76" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B77" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B78" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B79" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B80" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B81" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B82" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B83" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B84" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B85" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B86" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B87" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B88" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B89" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B90" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B91" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B92" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B93" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B94" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B95" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B96" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B97" t="s">
+        <v>99</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>